<commit_message>
Updated a note to be more descriptive
</commit_message>
<xml_diff>
--- a/Exercise Files/01_05.xlsx
+++ b/Exercise Files/01_05.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://quintiles-my.sharepoint.com/personal/mdmuntaha_islam_iqvia_com/Documents/Documents/My Courses/Data-Analytics-for-Business-Professionals/Exercise Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="11_407AE5EB0E4FDEEA21EFB05D0A1CB055DF79EF4C" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{ECF3B8B6-5D17-4E41-BD37-B0917B8C6325}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="11_407AE5EB0E4FDEEA21EFB05D0A1CB055DF79EF4C" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{850E0B65-B440-428E-960E-56184F9F0A9E}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -235,7 +235,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Middle number in an ascending ordered series.</t>
+Middle number in an ascending ordered series. When the mean and the median are really close, it means the data has a normal distribution. Otherwise it's skewed. For this table, it can be said that it's skewed.</t>
         </r>
       </text>
     </comment>

</xml_diff>